<commit_message>
Added Dada with Account file
</commit_message>
<xml_diff>
--- a/ExcelFiles/Account.xlsx
+++ b/ExcelFiles/Account.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Acc" sheetId="1" r:id="rId1"/>
     <sheet name="Customer" sheetId="2" r:id="rId2"/>
     <sheet name="New Customer" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
   <si>
     <t>Row id</t>
   </si>
@@ -136,6 +137,24 @@
   </si>
   <si>
     <t>Piler1</t>
+  </si>
+  <si>
+    <t>Row_10</t>
+  </si>
+  <si>
+    <t>Row_11</t>
+  </si>
+  <si>
+    <t>Row_12</t>
+  </si>
+  <si>
+    <t>Row_13</t>
+  </si>
+  <si>
+    <t>Row_14</t>
+  </si>
+  <si>
+    <t>Row_15</t>
   </si>
 </sst>
 </file>
@@ -477,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" activeCellId="1" sqref="C12:C14 C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,6 +616,63 @@
       </c>
       <c r="C10" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -675,7 +751,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B2" sqref="A2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,4 +807,59 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>